<commit_message>
update genetics, cgm, eeg
</commit_message>
<xml_diff>
--- a/src/test/resources/CGM.xlsx
+++ b/src/test/resources/CGM.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>CA-X6O6AEL5</t>
+  </si>
+  <si>
+    <t>CA-31LWURJY</t>
+  </si>
+  <si>
+    <t>CA-5Q21FZ1X</t>
+  </si>
+  <si>
+    <t>CA-756V081T</t>
   </si>
 </sst>
 </file>
@@ -579,7 +588,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>

</xml_diff>